<commit_message>
kanban link in excel
</commit_message>
<xml_diff>
--- a/Notes/Hydrosens-link.xlsx
+++ b/Notes/Hydrosens-link.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trist\4A\HydroSens\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projets_DATA\HydroSensMDE\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A814D402-DCD5-4CC3-96F7-CF28D3792013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BC47A7-BD58-4793-81B2-B2DA7140C15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Resources</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Kanban model</t>
+  </si>
+  <si>
+    <t>https://www.canva.com/design/DAFdcfvUnxU/WSismOO5mmrhMfZfhGy6sA/edit?utm_content=DAFdcfvUnxU&amp;utm_campaign=designshare&amp;utm_medium=link2&amp;utm_source=sharebutton</t>
   </si>
 </sst>
 </file>
@@ -376,10 +379,10 @@
   <dimension ref="B2:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="108.6640625" customWidth="1"/>
@@ -410,7 +413,9 @@
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>